<commit_message>
Com tempo de cada tarefa
</commit_message>
<xml_diff>
--- a/Organizacao/Planilhas/Histórias Product Backlog.xlsx
+++ b/Organizacao/Planilhas/Histórias Product Backlog.xlsx
@@ -13,10 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="106">
-  <si>
-    <t>ID História</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
   <si>
     <t>História do Usuário</t>
   </si>
@@ -27,10 +24,6 @@
     <t>Como apostador,
 preciso cadastrar minha conta com meus Dados
 para utilizar dentro do sistema</t>
-  </si>
-  <si>
-    <t>BDD
-(Cenários de testes)</t>
   </si>
   <si>
     <t>Finalizado</t>
@@ -86,6 +79,16 @@
 para utilizacao da plataforma</t>
   </si>
   <si>
+    <t>http://www.pudim.com.br/</t>
+  </si>
+  <si>
+    <t>ID História</t>
+  </si>
+  <si>
+    <t>BDD
+(Cenários de testes)</t>
+  </si>
+  <si>
     <t>RNF Associados</t>
   </si>
   <si>
@@ -113,13 +116,13 @@
     <t>Diferenca</t>
   </si>
   <si>
-    <t>http://www.pudim.com.br/</t>
-  </si>
-  <si>
     <t>Cenário 1: Cadastro de torneio 
 Dado: Dados do torneio a ser cadastrado
 Quando: Quando for registrar as partidas
 entao: permitir a insercao de Dados e cadastrar as partidas</t>
+  </si>
+  <si>
+    <t>Acessibilidade</t>
   </si>
   <si>
     <t>Cenário 1: Algum ou todos os Dados de entrada invalidos
@@ -129,27 +132,11 @@
  E nao aceitar o cadastro</t>
   </si>
   <si>
-    <t>Acessibilidade</t>
-  </si>
-  <si>
     <t>Usabilidade</t>
-  </si>
-  <si>
-    <t>Concluir as tarefas que não foram
-concluídas na última sprint</t>
   </si>
   <si>
     <t>Criar o modelo conceitual
 do banco de Dados</t>
-  </si>
-  <si>
-    <t>Cenário 2: Dados incorretos
-Dados: Dados do torneio incorretos
-Quando: Quando for cadastrar as partidas
-Então: permitir a alteracão dos Dados</t>
-  </si>
-  <si>
-    <t>Fazer a Logo do Site</t>
   </si>
   <si>
     <t>Cenário 2: Dados corretos 
@@ -160,51 +147,11 @@
 E informa o usuario do sucesso do cadastro</t>
   </si>
   <si>
-    <t>Cenário 3: Limpar a tela
-Dados: botão de limpar
-Quando: algum torneio for desejado fazer a limpeza
-Então: permitir a limpeza da tela</t>
-  </si>
-  <si>
-    <t>CSS - Cabeçalho - 
-Colocar o cabeçalho na parte
-superior da tela</t>
-  </si>
-  <si>
-    <t>Cenário 4: Cadastro de jogos dentro de um torneio
-Dados: partidas do campeonato
-Quando: for cadastrado um torneio
-então permitir o registro de partidas</t>
-  </si>
-  <si>
-    <t>Funcionalidade</t>
-  </si>
-  <si>
-    <t>CSS - Fazer a estiliação para a
-tela de cadastro de torneios</t>
-  </si>
-  <si>
     <t>Segurança</t>
-  </si>
-  <si>
-    <t>Cenário 5: Permitir a alteracão de partidas
-Dados: data/hora, equipes participantes e ou Dados das partidas
-Quando: precisar alterar as partidas
-Então: permitir a alteracão das partidas</t>
-  </si>
-  <si>
-    <t>CSS - Fazer a estiliação para a
-tela de cadastro de partidas</t>
   </si>
   <si>
     <t>Criar o modelo lógico 
 do banco de Dados</t>
-  </si>
-  <si>
-    <t>Cenário 6: Tentativa de acesso ao perfil
-Dado:clicar na foto no canto superior esquerdo
-Quando: na procura pr uma partida
-Então: redirecionar para tela de perfil do usuario</t>
   </si>
   <si>
     <t>Cenário 3: Tentativa de invasao do sistema 
@@ -218,21 +165,6 @@
 do banco de Dados</t>
   </si>
   <si>
-    <t>Back End - Fazer a
-página de ADM</t>
-  </si>
-  <si>
-    <t>Cenário 7: Pressionar o botao de sair
-Dado: clicar no botao
-Quando: quiser desconectar sua conta do site
-entao: retornar a tela principal
-e: sem estar conectado a sua conta</t>
-  </si>
-  <si>
-    <t>CSS- Criar CSS para a página
-de ADM</t>
-  </si>
-  <si>
     <t>Cenário 4: Cancelar o cadastro
 Dado: Selecionar a opcao de cancelar cadastro
 Quando: no cadastro
@@ -244,39 +176,6 @@
 do banco de Dados</t>
   </si>
   <si>
-    <t>Cenário 1: Cadastro de torneio 
-Dado: Dados do torneio a ser cadastrado
-Quando: Quando for registrar o torneio
-entao: permitir a insercao de Dados e cadastrar o torneio</t>
-  </si>
-  <si>
-    <t>Back End - Criar página para 
-atualização dos resultados das 
-partidas</t>
-  </si>
-  <si>
-    <t>Cenário 2: Dados incorretos
-Dados: Dados do torneio incorretos
-Quando: Quando for cadastrar o torneio
-Então: permitir a alteracão dos Dados</t>
-  </si>
-  <si>
-    <t>CSS - Fazer o CSS para a tela de
-atulização de resultados das
-partidas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Back End - Página Principal -
-Seleção de Games - 
-</t>
-  </si>
-  <si>
-    <t>Cenário 4: Tentativa de acesso ao perfil
-Dado:clicar na foto no canto superior esquerdo
-Quando: na procura pr uma partida
-Então: redirecionar para tela de perfil do usuario</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cenário 1: Email ou senha incorretos
 Dado: Email ou senha incorretos
 Quando: na confirmacao do login
@@ -285,23 +184,8 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Back End - Páginda Princial - 
-Seleção de campeonatos </t>
-  </si>
-  <si>
     <t xml:space="preserve">Prototipacão das telas inciais
 </t>
-  </si>
-  <si>
-    <t>Cenário 5: pressionar o botao de sair
-Dado: clicar no botao
-Quando: quiser desconectar sua conta do site
-entao: retornar a tela principal
-e: sem estar conectado a sua conta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Back End - Página Principal -
-Visualização de partidas </t>
   </si>
   <si>
     <t>Cenário 2: Todos os Dados de entrada validos 
@@ -323,20 +207,8 @@
 e: retornar a tela de login sem acessar</t>
   </si>
   <si>
-    <t>Cenário 1:Tentativa de acesso a um jogo do sistema 
-Dado: Clicar em algum jogo mostrado na lista,
-Quando: Na procura por uma partida
-entâo: exibir ao usuário lista de campeonatos e partidas
-daquele jogo em específico</t>
-  </si>
-  <si>
     <t>Fazer verificacão dos campos para 
 a tela de cadastros</t>
-  </si>
-  <si>
-    <t>CSS - Página Principal -
-Listar todos os eSports disponíveis
-na parte esquerda do site</t>
   </si>
   <si>
     <t xml:space="preserve">Cenário 4: Esqueci minha senha 
@@ -348,6 +220,166 @@
   <si>
     <t>Fazer o tratamento de excecoes
 para a tela de cadastros de usuarios</t>
+  </si>
+  <si>
+    <t>Cenário 5: Cadastro
+Dado: selecionar a opcao de cadastrar
+Quando: Quando SELECIONAR O CADASTRO
+entao: redirecionar para a TELA DE CADASTROOOO</t>
+  </si>
+  <si>
+    <t>Criar o formulários
+para a tela de login</t>
+  </si>
+  <si>
+    <t>Como administrador,
+preciso de um ambiente especial 
+para cadastrar partidas e campeonatos oficiais</t>
+  </si>
+  <si>
+    <t>Cenário 1: Cadastro de torneio 
+Dado: Dados do torneio a ser cadastrado
+Quando: Quando for registrar o torneio
+entao: permitir a insercao de Dados e cadastrar o torneio</t>
+  </si>
+  <si>
+    <t>Fazer verificacão dos campos para 
+a tela de login</t>
+  </si>
+  <si>
+    <t>Cenário 2: Dados incorretos
+Dados: Dados do torneio incorretos
+Quando: Quando for cadastrar o torneio
+Então: permitir a alteracão dos Dados</t>
+  </si>
+  <si>
+    <t>Fazer tratamento de execoes para 
+a tela de login</t>
+  </si>
+  <si>
+    <t>Cenário 3: Limpar a tela
+Dados: botão de limpar
+Quando: algum torneio for desejado fazer a limpeza
+Então: permitir a limpeza da tela</t>
+  </si>
+  <si>
+    <t>Criar o formulários 
+para a tela de cadastros de equipes</t>
+  </si>
+  <si>
+    <t>Cenário 4: Cadastro de jogos dentro de um torneio
+Dados: partidas do campeonato
+Quando: for cadastrado um torneio
+então permitir o registro de partidas</t>
+  </si>
+  <si>
+    <t>fazer verificacão 
+dos campos, para a tela
+de cadastros de equipes</t>
+  </si>
+  <si>
+    <t>Concluir as tarefas que não foram
+concluídas na última sprint</t>
+  </si>
+  <si>
+    <t>Cenário 2: Dados incorretos
+Dados: Dados do torneio incorretos
+Quando: Quando for cadastrar as partidas
+Então: permitir a alteracão dos Dados</t>
+  </si>
+  <si>
+    <t>Fazer a Logo do Site</t>
+  </si>
+  <si>
+    <t>CSS - Cabeçalho - 
+Colocar o cabeçalho na parte
+superior da tela</t>
+  </si>
+  <si>
+    <t>Funcionalidade</t>
+  </si>
+  <si>
+    <t>CSS - Fazer a estiliação para a
+tela de cadastro de torneios</t>
+  </si>
+  <si>
+    <t>Cenário 5: Permitir a alteracão de partidas
+Dados: data/hora, equipes participantes e ou Dados das partidas
+Quando: precisar alterar as partidas
+Então: permitir a alteracão das partidas</t>
+  </si>
+  <si>
+    <t>CSS - Fazer a estiliação para a
+tela de cadastro de partidas</t>
+  </si>
+  <si>
+    <t>Cenário 6: Tentativa de acesso ao perfil
+Dado:clicar na foto no canto superior esquerdo
+Quando: na procura pr uma partida
+Então: redirecionar para tela de perfil do usuario</t>
+  </si>
+  <si>
+    <t>Back End - Fazer a
+página de ADM</t>
+  </si>
+  <si>
+    <t>Cenário 7: Pressionar o botao de sair
+Dado: clicar no botao
+Quando: quiser desconectar sua conta do site
+entao: retornar a tela principal
+e: sem estar conectado a sua conta</t>
+  </si>
+  <si>
+    <t>CSS- Criar CSS para a página
+de ADM</t>
+  </si>
+  <si>
+    <t>Back End - Criar página para 
+atualização dos resultados das 
+partidas</t>
+  </si>
+  <si>
+    <t>CSS - Fazer o CSS para a tela de
+atulização de resultados das
+partidas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back End - Página Principal -
+Seleção de Games - 
+</t>
+  </si>
+  <si>
+    <t>Cenário 4: Tentativa de acesso ao perfil
+Dado:clicar na foto no canto superior esquerdo
+Quando: na procura pr uma partida
+Então: redirecionar para tela de perfil do usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back End - Páginda Princial - 
+Seleção de campeonatos </t>
+  </si>
+  <si>
+    <t>Cenário 5: pressionar o botao de sair
+Dado: clicar no botao
+Quando: quiser desconectar sua conta do site
+entao: retornar a tela principal
+e: sem estar conectado a sua conta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back End - Página Principal -
+Visualização de partidas </t>
+  </si>
+  <si>
+    <t>Cenário 1:Tentativa de acesso a um jogo do sistema 
+Dado: Clicar em algum jogo mostrado na lista,
+Quando: Na procura por uma partida
+entâo: exibir ao usuário lista de campeonatos e partidas
+daquele jogo em específico</t>
+  </si>
+  <si>
+    <t>CSS - Página Principal -
+Listar todos os eSports disponíveis
+na parte esquerda do site</t>
   </si>
   <si>
     <t>Cenário  2:selecionar um campeonato que nâo tem partidas cadastradas
@@ -362,16 +394,6 @@
 com mais apostas</t>
   </si>
   <si>
-    <t>Cenário 5: Cadastro
-Dado: selecionar a opcao de cadastrar
-Quando: Quando SELECIONAR O CADASTRO
-entao: redirecionar para a TELA DE CADASTROOOO</t>
-  </si>
-  <si>
-    <t>Criar o formulários
-para a tela de login</t>
-  </si>
-  <si>
     <t>Cenário 3: Tentativa de acesso ao perfil
 Dado:clicar na foto no canto superior esquerdo
 Quando: na procura pr uma partida
@@ -382,11 +404,6 @@
 Na direita inferior da tela
 colocar jogos
 recentemente acabados</t>
-  </si>
-  <si>
-    <t>Como administrador,
-preciso de um ambiente especial 
-para cadastrar partidas e campeonatos oficiais</t>
   </si>
   <si>
     <t>Cenário 4: pressionar o botao de sair
@@ -400,49 +417,9 @@
 Colocar os direitos do site</t>
   </si>
   <si>
-    <t>Fazer verificacão dos campos para 
-a tela de login</t>
-  </si>
-  <si>
-    <t>Fazer tratamento de execoes para 
-a tela de login</t>
-  </si>
-  <si>
-    <t>Criar o formulários 
-para a tela de cadastros de equipes</t>
-  </si>
-  <si>
-    <t>fazer verificacão 
-dos campos, para a tela
-de cadastros de equipes</t>
-  </si>
-  <si>
-    <t>Cenário 1: Tentativa de apostar
-Dado: clicar em apostar Quando escolhido uma partida
-Quando: quiser apostar 
-entao: exibir detalhes da aposta</t>
-  </si>
-  <si>
-    <t>Back End - Página Principal - 
-Ao selecionar a partida 
-redirecionar para a pagina
-da partida</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 fazer o tratamento de excecoes
 para a tela de cadastro de equipes</t>
-  </si>
-  <si>
-    <t>Cenário 2: ter uma confirmação na hora de apostar
-Dado: clicar no botão de apostar
-Quando: for confirmar a aposta
-Então: pedir uma confirmação ao usuário</t>
-  </si>
-  <si>
-    <t>Back End - Página da Partida - 
-Permiir que apostas sejam realizadas
-Na página da partida</t>
   </si>
   <si>
     <t>Como apostador, 
@@ -457,17 +434,6 @@
 entâo: redirecionar o usuario para a tela da partida</t>
   </si>
   <si>
-    <t>Cenário 3: ter uma confirmação de aposta realizada
-Dado: confrimar a apsota
-Quando: a apsota for confirmada
-Então: informar ao usuário que a aposta foi realizada</t>
-  </si>
-  <si>
-    <t>CSS - Página da Partida
-Fazer o CSS para a página
-da partida</t>
-  </si>
-  <si>
     <t>Criar o formulários 
 para a tela de cadastros de torneios</t>
   </si>
@@ -477,7 +443,7 @@
 para o cadastro de torneios</t>
   </si>
   <si>
-    <t>TOTAL:</t>
+    <t>-</t>
   </si>
   <si>
     <t>fazer o tratamento de excecoes
@@ -523,6 +489,43 @@
     <t xml:space="preserve">
 Definir padrão das telas (CSS)</t>
   </si>
+  <si>
+    <t>TOTAL:</t>
+  </si>
+  <si>
+    <t>Cenário 1: Tentativa de apostar
+Dado: clicar em apostar Quando escolhido uma partida
+Quando: quiser apostar 
+entao: exibir detalhes da aposta</t>
+  </si>
+  <si>
+    <t>Back End - Página Principal - 
+Ao selecionar a partida 
+redirecionar para a pagina
+da partida</t>
+  </si>
+  <si>
+    <t>Cenário 2: ter uma confirmação na hora de apostar
+Dado: clicar no botão de apostar
+Quando: for confirmar a aposta
+Então: pedir uma confirmação ao usuário</t>
+  </si>
+  <si>
+    <t>Back End - Página da Partida - 
+Permiir que apostas sejam realizadas
+Na página da partida</t>
+  </si>
+  <si>
+    <t>Cenário 3: ter uma confirmação de aposta realizada
+Dado: confrimar a apsota
+Quando: a apsota for confirmada
+Então: informar ao usuário que a aposta foi realizada</t>
+  </si>
+  <si>
+    <t>CSS - Página da Partida
+Fazer o CSS para a página
+da partida</t>
+  </si>
 </sst>
 </file>
 
@@ -536,18 +539,18 @@
     </font>
     <font/>
     <font>
-      <sz val="12.0"/>
-      <color rgb="FFFFFFFF"/>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
+      <sz val="12.0"/>
       <color rgb="FFFFFFFF"/>
     </font>
     <font>
       <sz val="12.0"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -669,68 +672,56 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -738,10 +729,25 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -750,13 +756,10 @@
     <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -820,11 +823,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="E2:G20" displayName="Table_1" id="1">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="E2:L20" displayName="Table_1" id="1">
+  <tableColumns count="8">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
     <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
   </tableColumns>
   <tableStyleInfo name="Sprint 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
   <extLst>
@@ -873,99 +881,99 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="B5" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B6" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="B7" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B8" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>7.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>8.0</v>
@@ -974,7 +982,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>9.0</v>
@@ -983,7 +991,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
         <v>10.0</v>
@@ -1076,8 +1084,8 @@
       <c r="C29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>26</v>
+      <c r="A30" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -5975,547 +5983,907 @@
   </cols>
   <sheetData>
     <row r="1" ht="44.25" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="L1" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="9">
+      <c r="A2" s="12">
         <v>1.0</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>3</v>
+      <c r="B2" s="13" t="s">
+        <v>2</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="16">
         <v>1.0</v>
       </c>
       <c r="F2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="H2" s="14">
+        <v>0.92</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K2" s="17">
+        <f t="shared" ref="K2:K25" si="1">SUM(H2:J2)</f>
+        <v>1.72</v>
+      </c>
+      <c r="L2" s="17">
+        <f t="shared" ref="L2:L25" si="2">G2-K2</f>
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="18"/>
+      <c r="C3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="18">
+      <c r="D3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="16">
         <v>2.0</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="19"/>
-      <c r="C3" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>44</v>
+      <c r="F3" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="G3" s="14">
         <v>2.0</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
+      <c r="H3" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="I3" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="J3" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K3" s="17">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="17">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="19"/>
-      <c r="C4" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="A4" s="18"/>
+      <c r="C4" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="16">
         <v>3.0</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G4" s="14">
         <v>2.0</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="H4" s="16">
+        <v>2.51</v>
+      </c>
+      <c r="I4" s="16">
+        <v>0.68</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K4" s="17">
+        <f t="shared" si="1"/>
+        <v>3.49</v>
+      </c>
+      <c r="L4" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.49</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="18">
+        <v>37</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="16">
         <v>4.0</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="G5" s="14">
         <v>3.0</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="H5" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="I5" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K5" s="17">
+        <f t="shared" si="1"/>
+        <v>4.7</v>
+      </c>
+      <c r="L5" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.7</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="29">
+      <c r="A6" s="24">
         <v>2.0</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>6</v>
+      <c r="B6" s="24" t="s">
+        <v>4</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="18">
+        <v>39</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="16">
         <v>5.0</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>61</v>
+      <c r="F6" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="G6" s="14">
         <v>2.0</v>
       </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="H6" s="16">
+        <v>2.83</v>
+      </c>
+      <c r="I6" s="16">
+        <v>0.92</v>
+      </c>
+      <c r="J6" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K6" s="17">
+        <f t="shared" si="1"/>
+        <v>4.05</v>
+      </c>
+      <c r="L6" s="17">
+        <f t="shared" si="2"/>
+        <v>-2.05</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="18">
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="16">
         <v>6.0</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>65</v>
+      <c r="F7" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="G7" s="14">
         <v>3.0</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="H7" s="16">
+        <v>0.58</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K7" s="17">
+        <f t="shared" si="1"/>
+        <v>1.23</v>
+      </c>
+      <c r="L7" s="17">
+        <f t="shared" si="2"/>
+        <v>1.77</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="18">
+        <v>43</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="16">
         <v>7.0</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="G8" s="14">
         <v>3.0</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="H8" s="16">
+        <v>1.37</v>
+      </c>
+      <c r="I8" s="16">
+        <v>0.37</v>
+      </c>
+      <c r="J8" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K8" s="17">
+        <f t="shared" si="1"/>
+        <v>2.04</v>
+      </c>
+      <c r="L8" s="17">
+        <f t="shared" si="2"/>
+        <v>0.96</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="18">
+        <v>45</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="16">
         <v>8.0</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="G9" s="14">
         <v>3.0</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
+      <c r="H9" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="I9" s="16">
+        <v>0.37</v>
+      </c>
+      <c r="J9" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K9" s="17">
+        <f t="shared" si="1"/>
+        <v>3.67</v>
+      </c>
+      <c r="L9" s="17">
+        <f t="shared" si="2"/>
+        <v>-0.67</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="18">
+        <v>47</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="16">
         <v>9.0</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>75</v>
+      <c r="F10" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="G10" s="14">
         <v>2.0</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="H10" s="16">
+        <v>1.33</v>
+      </c>
+      <c r="I10" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K10" s="17">
+        <f t="shared" si="1"/>
+        <v>1.68</v>
+      </c>
+      <c r="L10" s="17">
+        <f t="shared" si="2"/>
+        <v>0.32</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="29">
+      <c r="A11" s="24">
         <v>3.0</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>78</v>
+      <c r="B11" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="18">
+        <v>50</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="16">
         <v>10.0</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="G11" s="14">
         <v>3.0</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
+      <c r="H11" s="16">
+        <v>2.92</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0.48</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K11" s="17">
+        <f t="shared" si="1"/>
+        <v>3.7</v>
+      </c>
+      <c r="L11" s="17">
+        <f t="shared" si="2"/>
+        <v>-0.7</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="18">
+        <v>52</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="16">
         <v>11.0</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="G12" s="14">
         <v>2.0</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="H12" s="16">
+        <v>3.16</v>
+      </c>
+      <c r="I12" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="J12" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K12" s="17">
+        <f t="shared" si="1"/>
+        <v>3.71</v>
+      </c>
+      <c r="L12" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.71</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="18">
+        <v>54</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="16">
         <v>12.0</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>83</v>
+      <c r="F13" s="16" t="s">
+        <v>55</v>
       </c>
       <c r="G13" s="14">
         <v>2.0</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
+      <c r="H13" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="I13" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="J13" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K13" s="17">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L13" s="17">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="18">
+        <v>56</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="16">
         <v>13.0</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="G14" s="14">
         <v>2.0</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
+      <c r="H14" s="16">
+        <v>1.3</v>
+      </c>
+      <c r="I14" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K14" s="17">
+        <f t="shared" si="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="L14" s="17">
+        <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="18">
+        <v>64</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="16">
         <v>14.0</v>
       </c>
       <c r="F15" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="J15" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K15" s="17">
+        <f t="shared" si="1"/>
+        <v>0.34</v>
+      </c>
+      <c r="L15" s="17">
+        <f t="shared" si="2"/>
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="24">
+        <v>4.0</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="18">
+      <c r="D16" s="31"/>
+      <c r="E16" s="16">
+        <v>15.0</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="16">
         <v>2.0</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="29">
-        <v>4.0</v>
-      </c>
-      <c r="B16" s="29" t="s">
+      <c r="H16" s="16">
+        <v>1.25</v>
+      </c>
+      <c r="I16" s="16">
+        <v>2.92</v>
+      </c>
+      <c r="J16" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K16" s="17">
+        <f t="shared" si="1"/>
+        <v>4.47</v>
+      </c>
+      <c r="L16" s="17">
+        <f t="shared" si="2"/>
+        <v>-2.47</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="16">
+        <v>16.0</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="H17" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="I17" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="J17" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K17" s="17">
+        <f t="shared" si="1"/>
+        <v>0.63</v>
+      </c>
+      <c r="L17" s="17">
+        <f t="shared" si="2"/>
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="16">
+        <v>17.0</v>
+      </c>
+      <c r="F18" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="18">
-        <v>15.0</v>
-      </c>
-      <c r="F16" s="18" t="s">
+      <c r="G18" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="H18" s="16">
+        <v>2.35</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K18" s="17">
+        <f t="shared" si="1"/>
+        <v>2.65</v>
+      </c>
+      <c r="L18" s="17">
+        <f t="shared" si="2"/>
+        <v>-0.65</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="25"/>
+      <c r="E19" s="16">
+        <v>18.0</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="H19" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" si="1"/>
+        <v>3.8</v>
+      </c>
+      <c r="L19" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="16">
+        <v>19.0</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="18">
-        <v>16.0</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="G17" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="18">
-        <v>17.0</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="18">
-        <v>18.0</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="G19" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="18">
-        <v>19.0</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G20" s="18">
+      <c r="G20" s="16">
         <v>3.0</v>
       </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
+      <c r="H20" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K20" s="17">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="L20" s="17">
+        <f t="shared" si="2"/>
+        <v>2.7</v>
+      </c>
     </row>
     <row r="21">
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="14">
         <v>20.0</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="G21" s="18">
+        <v>95</v>
+      </c>
+      <c r="G21" s="16">
         <v>3.0</v>
       </c>
+      <c r="H21" s="14">
+        <v>2.38</v>
+      </c>
+      <c r="I21" s="14">
+        <v>0.53</v>
+      </c>
+      <c r="J21" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K21" s="17">
+        <f t="shared" si="1"/>
+        <v>3.21</v>
+      </c>
+      <c r="L21" s="17">
+        <f t="shared" si="2"/>
+        <v>-0.21</v>
+      </c>
     </row>
     <row r="22">
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
       <c r="E22" s="14">
         <v>21.0</v>
       </c>
-      <c r="F22" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="18">
+      <c r="F22" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" s="16">
         <v>3.0</v>
       </c>
+      <c r="H22" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K22" s="17">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="L22" s="17">
+        <f t="shared" si="2"/>
+        <v>2.7</v>
+      </c>
     </row>
     <row r="23">
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="14">
         <v>22.0</v>
       </c>
-      <c r="F23" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="18">
+      <c r="F23" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="16">
         <v>3.0</v>
       </c>
+      <c r="H23" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K23" s="17">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="L23" s="17">
+        <f t="shared" si="2"/>
+        <v>2.7</v>
+      </c>
     </row>
     <row r="24">
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="14">
         <v>23.0</v>
       </c>
-      <c r="F24" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="18">
+      <c r="F24" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="16">
         <v>2.0</v>
       </c>
+      <c r="H24" s="14">
+        <v>0.48</v>
+      </c>
+      <c r="I24" s="14">
+        <v>1.11</v>
+      </c>
+      <c r="J24" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K24" s="17">
+        <f t="shared" si="1"/>
+        <v>1.89</v>
+      </c>
+      <c r="L24" s="17">
+        <f t="shared" si="2"/>
+        <v>0.11</v>
+      </c>
     </row>
     <row r="25">
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="14">
         <v>24.0</v>
       </c>
-      <c r="F25" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="18">
+      <c r="F25" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" s="16">
         <v>3.0</v>
       </c>
+      <c r="H25" s="14">
+        <v>6.5</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="K25" s="17">
+        <f t="shared" si="1"/>
+        <v>6.8</v>
+      </c>
+      <c r="L25" s="17">
+        <f t="shared" si="2"/>
+        <v>-3.8</v>
+      </c>
     </row>
     <row r="26">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
       <c r="E26" s="33"/>
-      <c r="F26" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="34">
+      <c r="F26" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="17">
         <f>sum(G2:G25)</f>
         <v>58</v>
+      </c>
+      <c r="H26" s="33">
+        <f t="shared" ref="H26:L26" si="3">SUM(H2:H25)</f>
+        <v>41.88</v>
+      </c>
+      <c r="I26" s="33">
+        <f t="shared" si="3"/>
+        <v>12.25</v>
+      </c>
+      <c r="J26" s="33">
+        <f t="shared" si="3"/>
+        <v>7.2</v>
+      </c>
+      <c r="K26" s="33">
+        <f t="shared" si="3"/>
+        <v>61.33</v>
+      </c>
+      <c r="L26" s="33">
+        <f t="shared" si="3"/>
+        <v>-3.33</v>
       </c>
     </row>
   </sheetData>
@@ -6556,45 +6924,48 @@
     <col customWidth="1" min="4" max="4" width="17.86"/>
     <col customWidth="1" min="5" max="5" width="12.57"/>
     <col customWidth="1" min="6" max="6" width="38.43"/>
-    <col customWidth="1" min="8" max="8" width="17.57"/>
+    <col customWidth="1" min="7" max="7" width="17.71"/>
+    <col customWidth="1" min="8" max="8" width="20.86"/>
+    <col customWidth="1" min="9" max="9" width="14.86"/>
+    <col customWidth="1" min="10" max="10" width="17.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="44.25" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
@@ -6613,28 +6984,28 @@
       <c r="AA1" s="7"/>
     </row>
     <row r="2">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>1.0</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="15">
+      <c r="D2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="26">
         <v>1.0</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="15">
+      <c r="F2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="26">
         <v>2.5</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -6656,24 +7027,24 @@
       <c r="AA2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="15">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="26">
         <v>2.0</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="13">
+      <c r="F3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="11">
         <v>4.0</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -6695,24 +7066,24 @@
       <c r="AA3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="15">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="26">
         <v>3.0</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="15">
+      <c r="F4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="26">
         <v>2.75</v>
       </c>
-      <c r="H4" s="17"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -6734,24 +7105,24 @@
       <c r="AA4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="15">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="26">
         <v>4.0</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="F5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="11">
         <v>3.0</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -6773,24 +7144,24 @@
       <c r="AA5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="15">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="26">
         <v>5.0</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="13">
+      <c r="F6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="11">
         <v>2.5</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="27"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -6812,24 +7183,24 @@
       <c r="AA6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="15">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="26">
         <v>6.0</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="F7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="11">
         <v>1.75</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -6851,24 +7222,24 @@
       <c r="AA7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="15">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="26">
         <v>7.0</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="13">
+      <c r="F8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="11">
         <v>3.0</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="27"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -6890,28 +7261,28 @@
       <c r="AA8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>2.0</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="15">
+      <c r="B9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="26">
         <v>8.0</v>
       </c>
-      <c r="F9" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="15">
+      <c r="F9" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="26">
         <v>3.75</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="27"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
@@ -6933,24 +7304,24 @@
       <c r="AA9" s="7"/>
     </row>
     <row r="10">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="15">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="26">
         <v>9.0</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="15">
+      <c r="F10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="26">
         <v>2.0</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="27"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
@@ -6972,24 +7343,24 @@
       <c r="AA10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="15">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="26">
         <v>10.0</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="15">
+      <c r="F11" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="26">
         <v>3.0</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="27"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
@@ -7011,24 +7382,24 @@
       <c r="AA11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="15">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="26">
         <v>11.0</v>
       </c>
-      <c r="F12" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="15">
+      <c r="F12" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="26">
         <v>3.0</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="27"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -7050,24 +7421,24 @@
       <c r="AA12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="24" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="15">
+      <c r="E13" s="26">
         <v>12.0</v>
       </c>
-      <c r="F13" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="15">
+      <c r="F13" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="26">
         <v>3.0</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="27"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -7089,28 +7460,28 @@
       <c r="AA13" s="7"/>
     </row>
     <row r="14">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
         <v>3.0</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="15">
+      <c r="B14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="26">
         <v>13.0</v>
       </c>
-      <c r="F14" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="15">
+      <c r="F14" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="26">
         <v>5.5</v>
       </c>
-      <c r="H14" s="17"/>
+      <c r="H14" s="27"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
@@ -7132,24 +7503,24 @@
       <c r="AA14" s="7"/>
     </row>
     <row r="15">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="15">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="26">
         <v>14.0</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="15">
+      <c r="F15" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="26">
         <v>3.0</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="27"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -7171,24 +7542,24 @@
       <c r="AA15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="15">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="26">
         <v>15.0</v>
       </c>
-      <c r="F16" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="15">
+      <c r="F16" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="26">
         <v>3.0</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="27"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
@@ -7210,24 +7581,24 @@
       <c r="AA16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="15">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="26">
         <v>16.0</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="15">
+      <c r="F17" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="26">
         <v>1.5</v>
       </c>
-      <c r="H17" s="17"/>
+      <c r="H17" s="27"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -7249,28 +7620,28 @@
       <c r="AA17" s="7"/>
     </row>
     <row r="18">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>4.0</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="15">
+      <c r="B18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="26">
         <v>17.0</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" s="15">
+      <c r="F18" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="26">
         <v>3.0</v>
       </c>
-      <c r="H18" s="17"/>
+      <c r="H18" s="27"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
@@ -7292,24 +7663,24 @@
       <c r="AA18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="15">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="26">
         <v>18.0</v>
       </c>
-      <c r="F19" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="15">
+      <c r="F19" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="26">
         <v>3.0</v>
       </c>
-      <c r="H19" s="17"/>
+      <c r="H19" s="27"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -7331,24 +7702,24 @@
       <c r="AA19" s="7"/>
     </row>
     <row r="20">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="15">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="26">
         <v>19.0</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" s="15">
+      <c r="F20" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G20" s="26">
         <v>3.75</v>
       </c>
-      <c r="H20" s="17"/>
+      <c r="H20" s="27"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
@@ -7370,19 +7741,19 @@
       <c r="AA20" s="7"/>
     </row>
     <row r="21">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="15">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="26">
         <v>20.0</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="17"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="27"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
@@ -7404,20 +7775,20 @@
       <c r="AA21" s="7"/>
     </row>
     <row r="22">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="24" t="s">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="15">
+      <c r="E22" s="26">
         <v>21.0</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="17"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="27"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
@@ -7443,13 +7814,13 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="15">
+      <c r="E23" s="26">
         <v>22.0</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="32">
+      <c r="F23" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="34">
         <f>SUM(G2:G22)</f>
         <v>57</v>
       </c>

</xml_diff>